<commit_message>
Add DK value to distanceTables
</commit_message>
<xml_diff>
--- a/server-loader/prototype-clustering/community_module/similarity/distanceTables/beliefE.xlsx
+++ b/server-loader/prototype-clustering/community_module/similarity/distanceTables/beliefE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\root\WORK\python\20221017\community-model-api\server-loader\prototype-clustering\community_module\similarity\distanceTables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\root\WORK\python\20221114\community-model-api\server-loader\prototype-clustering\community_module\similarity\distanceTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="7">
   <si>
     <t>NotTraitor</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>1.0</t>
+  </si>
+  <si>
+    <t>DK</t>
   </si>
 </sst>
 </file>
@@ -853,10 +856,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -864,7 +867,7 @@
     <col min="2" max="4" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -874,8 +877,11 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -888,8 +894,11 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -902,8 +911,11 @@
       <c r="D3" t="s">
         <v>4</v>
       </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -914,6 +926,26 @@
         <v>4</v>
       </c>
       <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>